<commit_message>
added equivalencies to dataset
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/worklearn/Documents/course-mapper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2A1FB08-C489-7849-8139-6583A1165FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EDE1F1-F244-0D42-A30B-665E38990E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="740" windowWidth="38400" windowHeight="21800" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="requisites_program1" sheetId="8" r:id="rId8"/>
     <sheet name="courses_program2" sheetId="10" r:id="rId9"/>
     <sheet name="requisites_program2" sheetId="11" r:id="rId10"/>
-    <sheet name="tracks" sheetId="9" r:id="rId11"/>
-    <sheet name="reflections" sheetId="12" r:id="rId12"/>
+    <sheet name="equivalencies" sheetId="13" r:id="rId11"/>
+    <sheet name="tracks" sheetId="9" r:id="rId12"/>
+    <sheet name="reflections" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="301">
   <si>
     <t>course_number</t>
   </si>
@@ -893,6 +894,60 @@
   <si>
     <t>›</t>
   </si>
+  <si>
+    <t>equivalency_id</t>
+  </si>
+  <si>
+    <t>equivalency_number</t>
+  </si>
+  <si>
+    <t>M102</t>
+  </si>
+  <si>
+    <t>M104</t>
+  </si>
+  <si>
+    <t>M110</t>
+  </si>
+  <si>
+    <t>M120</t>
+  </si>
+  <si>
+    <t>M180</t>
+  </si>
+  <si>
+    <t>M184</t>
+  </si>
+  <si>
+    <t>M103</t>
+  </si>
+  <si>
+    <t>M105</t>
+  </si>
+  <si>
+    <t>M121</t>
+  </si>
+  <si>
+    <t>M152</t>
+  </si>
+  <si>
+    <t>M223</t>
+  </si>
+  <si>
+    <t>M302</t>
+  </si>
+  <si>
+    <t>M226</t>
+  </si>
+  <si>
+    <t>M217</t>
+  </si>
+  <si>
+    <t>M253</t>
+  </si>
+  <si>
+    <t>M254</t>
+  </si>
 </sst>
 </file>
 
@@ -901,7 +956,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -956,6 +1011,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2847,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5775,6 +5836,213 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A069C6A7-B946-D341-8999-6171849D292F}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
@@ -6909,7 +7177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -36777,7 +37045,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D55"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>